<commit_message>
instrumentAttribute version at the time of data upload
</commit_message>
<xml_diff>
--- a/docs/SubledgerE2E_Aggregation_Testing_Activity_D2.xlsx
+++ b/docs/SubledgerE2E_Aggregation_Testing_Activity_D2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="InstrumentAttribute" sheetId="1" state="visible" r:id="rId3"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="72">
   <si>
     <t xml:space="preserve">EffectiveDate</t>
   </si>
@@ -91,9 +91,6 @@
     <t xml:space="preserve">OriginalFICOScore</t>
   </si>
   <si>
-    <t xml:space="preserve">30/04/2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">LOAN1</t>
   </si>
   <si>
@@ -115,7 +112,7 @@
     <t xml:space="preserve">ACCRUAL</t>
   </si>
   <si>
-    <t xml:space="preserve">30/06/2024</t>
+    <t xml:space="preserve">LOAN2</t>
   </si>
   <si>
     <t xml:space="preserve">TransactionDate</t>
@@ -125,9 +122,6 @@
   </si>
   <si>
     <t xml:space="preserve">Amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOAN2</t>
   </si>
   <si>
     <t xml:space="preserve">Disburse Principal-Principal</t>
@@ -350,15 +344,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -647,235 +641,294 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K29" activeCellId="1" sqref="A:A K29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.39"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
+        <v>45412</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="B2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>45292</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="2" t="n">
-        <v>45292</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="3" t="n">
+        <v>45658</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="2" t="n">
-        <v>45658</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="2" t="n">
+      <c r="J2" s="3" t="n">
         <v>45323</v>
       </c>
-      <c r="K2" s="3" t="n">
+      <c r="K2" s="1" t="n">
         <v>12</v>
       </c>
       <c r="L2" s="6" t="n">
         <v>102</v>
       </c>
       <c r="M2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="1"/>
+      <c r="S2" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="T2" s="1"/>
+      <c r="U2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3" t="n">
+      <c r="V2" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <f aca="false">A2</f>
+        <v>45412</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>45292</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>45658</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>45323</v>
+      </c>
+      <c r="K3" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="T2" s="3"/>
-      <c r="U2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="V2" s="3" t="n">
+      <c r="L3" s="6" t="n">
+        <v>102</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V3" s="1" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="4" t="n">
-        <f aca="false">B2</f>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>45473</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <f aca="false">B3</f>
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="str">
-        <f aca="false">C2</f>
-        <v>LOAN1</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <f aca="false">D2</f>
+      <c r="C4" s="1" t="str">
+        <f aca="false">C3</f>
+        <v>LOAN2</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <f aca="false">D3</f>
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="str">
-        <f aca="false">E2</f>
+      <c r="E4" s="1" t="str">
+        <f aca="false">E3</f>
         <v>Revolving</v>
       </c>
-      <c r="F3" s="2" t="n">
-        <f aca="false">F2</f>
+      <c r="F4" s="3" t="n">
+        <f aca="false">F3</f>
         <v>45292</v>
       </c>
-      <c r="G3" s="3" t="str">
-        <f aca="false">G2</f>
+      <c r="G4" s="1" t="str">
+        <f aca="false">G3</f>
         <v>Origination</v>
       </c>
-      <c r="H3" s="2" t="n">
-        <f aca="false">H2</f>
+      <c r="H4" s="3" t="n">
+        <f aca="false">H3</f>
         <v>45658</v>
       </c>
-      <c r="I3" s="3" t="str">
-        <f aca="false">I2</f>
+      <c r="I4" s="1" t="str">
+        <f aca="false">I3</f>
         <v>PRINCIPAL_AND_INTEREST</v>
       </c>
-      <c r="J3" s="2" t="n">
-        <f aca="false">J2</f>
+      <c r="J4" s="3" t="n">
+        <f aca="false">J3</f>
         <v>45323</v>
       </c>
-      <c r="K3" s="3" t="n">
-        <f aca="false">K2</f>
+      <c r="K4" s="1" t="n">
+        <f aca="false">K3</f>
         <v>12</v>
       </c>
-      <c r="L3" s="7" t="n">
+      <c r="L4" s="7" t="n">
         <v>103</v>
       </c>
-      <c r="M3" s="3" t="str">
-        <f aca="false">M2</f>
+      <c r="M4" s="1" t="str">
+        <f aca="false">M3</f>
         <v>ABC</v>
       </c>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="4" t="str">
-        <f aca="false">Q2</f>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="4" t="str">
+        <f aca="false">Q3</f>
         <v>FAS91</v>
       </c>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3" t="n">
-        <f aca="false">S2</f>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1" t="n">
+        <f aca="false">S3</f>
         <v>12</v>
       </c>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3" t="str">
-        <f aca="false">U2</f>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1" t="str">
+        <f aca="false">U3</f>
         <v>ACCRUAL</v>
       </c>
-      <c r="V3" s="3" t="n">
-        <f aca="false">V2</f>
+      <c r="V4" s="1" t="n">
+        <f aca="false">V3</f>
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="8"/>
-    </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="8"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -894,49 +947,48 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="24.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="18.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="35.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="22.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>33</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="XFD1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="n">
         <v>45412</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="12" t="n">
         <v>200000</v>
@@ -944,7 +996,6 @@
       <c r="E2" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="XFD2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="n">
@@ -956,7 +1007,7 @@
         <v>LOAN2</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" s="12" t="n">
         <v>2400</v>
@@ -964,7 +1015,6 @@
       <c r="E3" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="XFD3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="n">
@@ -975,7 +1025,7 @@
         <v>LOAN2</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" s="12" t="n">
         <v>200</v>
@@ -984,7 +1034,6 @@
         <v>1</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="XFD4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="n">
@@ -996,7 +1045,7 @@
         <v>LOAN2</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D5" s="12" t="n">
         <v>1000</v>
@@ -1005,7 +1054,6 @@
         <v>1</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="XFD5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="n">
@@ -1016,7 +1064,7 @@
         <v>LOAN2</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6" s="12" t="n">
         <v>200</v>
@@ -1025,7 +1073,6 @@
         <v>1</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="XFD6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="n">
@@ -1037,7 +1084,7 @@
         <v>LOAN2</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" s="12" t="n">
         <v>100</v>
@@ -1046,7 +1093,6 @@
         <v>1</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="XFD7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="n">
@@ -1058,7 +1104,7 @@
         <v>LOAN2</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D8" s="12" t="n">
         <v>100</v>
@@ -1067,7 +1113,6 @@
         <v>1</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="XFD8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="n">
@@ -1079,7 +1124,7 @@
         <v>LOAN2</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D9" s="12" t="n">
         <v>100</v>
@@ -1088,135 +1133,118 @@
         <v>1</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="XFD9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
+      <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="XFD10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
+      <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="XFD11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="XFD12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="XFD13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2"/>
+      <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="XFD14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2"/>
+      <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="XFD15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2"/>
+      <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="XFD16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2"/>
+      <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="XFD17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2"/>
+      <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="XFD18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2"/>
+      <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="XFD19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2"/>
+      <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-      <c r="XFD20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2"/>
+      <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="XFD21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2"/>
+      <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="XFD22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2"/>
+      <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="XFD23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2"/>
+      <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-      <c r="XFD24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2"/>
+      <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-      <c r="XFD25" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1238,296 +1266,296 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="1" sqref="A:A B28"/>
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="57.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="34.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="57.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="str">
+      <c r="A3" s="1" t="str">
         <f aca="false">CONCATENATE(C3,F3,E3)</f>
         <v>Revenueamount&gt;1Dr</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="str">
+      <c r="A4" s="1" t="str">
         <f aca="false">CONCATENATE(C4,F4,E4)</f>
         <v>Revenueamount&gt;1Cr</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="str">
+      <c r="A5" s="1" t="str">
         <f aca="false">CONCATENATE(C5,F5,E5)</f>
         <v>Revenueamount&lt;1Dr</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>51</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="str">
+      <c r="A6" s="1" t="str">
         <f aca="false">CONCATENATE(C6,F6,E6)</f>
         <v>Revenueamount&lt;1Cr</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="C6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="str">
+      <c r="A7" s="1" t="str">
         <f aca="false">CONCATENATE(C7,F7,E7)</f>
         <v>Deferred Revenueamount&gt;1Dr</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="str">
+      <c r="A8" s="1" t="str">
         <f aca="false">CONCATENATE(C8,F8,E8)</f>
         <v>Deferred Revenueamount&gt;1Cr</v>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="str">
+      <c r="A9" s="1" t="str">
         <f aca="false">CONCATENATE(C9,F9,E9)</f>
         <v>Deferred Revenueamount&lt;1Dr</v>
       </c>
-      <c r="B9" s="3" t="n">
+      <c r="B9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>55</v>
+      <c r="D9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="str">
+      <c r="A10" s="1" t="str">
         <f aca="false">CONCATENATE(C10,F10,E10)</f>
         <v>Deferred Revenueamount&lt;1Cr</v>
       </c>
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="str">
+      <c r="A11" s="1" t="str">
         <f aca="false">CONCATENATE(C11,F11,E11)</f>
         <v>A/Ramount&gt;1Dr</v>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="C11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="str">
+      <c r="A12" s="1" t="str">
         <f aca="false">CONCATENATE(C12,F12,E12)</f>
         <v>A/Ramount&gt;1Cr</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="C12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="str">
+      <c r="A13" s="1" t="str">
         <f aca="false">CONCATENATE(C13,F13,E13)</f>
         <v>A/Ramount&lt;1Dr</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="D13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="str">
+      <c r="A14" s="1" t="str">
         <f aca="false">CONCATENATE(C14,F14,E14)</f>
         <v>A/Ramount&lt;1Cr</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="C14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="str">
+      <c r="A15" s="1" t="str">
         <f aca="false">CONCATENATE(C15,D15,E15)</f>
         <v/>
       </c>
@@ -1551,7 +1579,7 @@
   <dimension ref="B1:O25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q20" activeCellId="1" sqref="A:A Q20"/>
+      <selection pane="topLeft" activeCell="Q20" activeCellId="0" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1560,53 +1588,53 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="3" t="n">
+      <c r="B1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="D2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="3" t="s">
+      <c r="H2" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="1" t="n">
         <v>-100</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>49</v>
+      <c r="G3" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="4" t="str">
@@ -1618,33 +1646,33 @@
       </c>
       <c r="E5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="n">
         <v>-100</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D8" s="4" t="n">
         <v>200</v>
@@ -1652,15 +1680,15 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="n">
@@ -1668,60 +1696,60 @@
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="M10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="N10" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="O10" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="N10" s="4" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="O10" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="H11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="O11" s="1" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="3" t="n">
-        <v>200</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="M11" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="O11" s="3" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="3" t="n">
+      <c r="E12" s="1" t="n">
         <v>-200</v>
       </c>
       <c r="G12" s="4" t="str">
@@ -1729,13 +1757,13 @@
         <v>Revenue</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J12" s="4" t="n">
         <f aca="false">O11</f>
         <v>100</v>
       </c>
-      <c r="M12" s="3" t="n">
+      <c r="M12" s="1" t="n">
         <v>100</v>
       </c>
       <c r="O12" s="4" t="n">
@@ -1748,35 +1776,35 @@
         <f aca="false">O12</f>
         <v>200</v>
       </c>
-      <c r="L13" s="3" t="n">
+      <c r="L13" s="1" t="n">
         <v>1200</v>
       </c>
-      <c r="M13" s="3" t="n">
+      <c r="M13" s="1" t="n">
         <v>100</v>
       </c>
       <c r="N13" s="4" t="n">
         <f aca="false">L13-J13-M13</f>
         <v>900</v>
       </c>
-      <c r="O13" s="3" t="n">
+      <c r="O13" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="3" t="n">
+      <c r="C14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="1" t="n">
         <v>1200</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>72</v>
+      <c r="G14" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K14" s="4" t="n">
         <f aca="false">N13</f>
@@ -1791,10 +1819,10 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="3" t="n">
+      <c r="C15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="1" t="n">
         <v>-1200</v>
       </c>
       <c r="G15" s="4" t="str">
@@ -1802,7 +1830,7 @@
         <v>Def Revenue</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K15" s="4" t="n">
         <f aca="false">N14</f>
@@ -1832,20 +1860,20 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="3" t="n">
+      <c r="B17" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="3" t="n">
+      <c r="C17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="1" t="n">
         <v>100</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K17" s="4" t="n">
         <f aca="false">N16</f>
@@ -1861,10 +1889,10 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="3" t="n">
+      <c r="C18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="1" t="n">
         <v>-100</v>
       </c>
       <c r="G18" s="4" t="str">
@@ -1872,7 +1900,7 @@
         <v>Revenue</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K18" s="4" t="n">
         <f aca="false">N17</f>
@@ -1916,17 +1944,17 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="3" t="s">
+      <c r="C21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>70</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="K21" s="4" t="n">
         <f aca="false">N20</f>
@@ -1942,21 +1970,21 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="3" t="n">
+      <c r="B22" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C22" s="3" t="n">
+      <c r="C22" s="1" t="n">
         <f aca="false">D2</f>
         <v>100</v>
       </c>
-      <c r="D22" s="3" t="n">
+      <c r="D22" s="1" t="n">
         <f aca="false">E3</f>
         <v>-100</v>
       </c>
-      <c r="E22" s="3" t="n">
+      <c r="E22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F22" s="3" t="n">
+      <c r="F22" s="1" t="n">
         <v>0</v>
       </c>
       <c r="K22" s="4" t="n">
@@ -1973,53 +2001,53 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="3" t="n">
+      <c r="B23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C23" s="3" t="n">
+      <c r="C23" s="1" t="n">
         <f aca="false">D5</f>
         <v>100</v>
       </c>
-      <c r="D23" s="3" t="n">
+      <c r="D23" s="1" t="n">
         <f aca="false">E6</f>
         <v>-100</v>
       </c>
-      <c r="E23" s="3" t="n">
+      <c r="E23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F23" s="3" t="n">
+      <c r="F23" s="1" t="n">
         <v>0</v>
       </c>
       <c r="G23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="3" t="n">
+      <c r="B24" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C24" s="3" t="n">
+      <c r="C24" s="1" t="n">
         <f aca="false">E9</f>
         <v>-200</v>
       </c>
-      <c r="D24" s="3" t="n">
+      <c r="D24" s="1" t="n">
         <f aca="false">D8+E12+E18</f>
         <v>-100</v>
       </c>
-      <c r="E24" s="3" t="n">
+      <c r="E24" s="1" t="n">
         <f aca="false">D14</f>
         <v>1200</v>
       </c>
-      <c r="F24" s="3" t="n">
+      <c r="F24" s="1" t="n">
         <f aca="false">D11+E15+D17</f>
         <v>-900</v>
       </c>
       <c r="G24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="3" t="n">
+      <c r="C25" s="1" t="n">
         <f aca="false">SUM(C22:C24)</f>
         <v>0</v>
       </c>
-      <c r="D25" s="3" t="n">
+      <c r="D25" s="1" t="n">
         <f aca="false">SUM(D22:D24)</f>
         <v>-300</v>
       </c>

</xml_diff>